<commit_message>
mise à jour nouvelle
</commit_message>
<xml_diff>
--- a/Mon Code/topic_analysis.xlsx
+++ b/Mon Code/topic_analysis.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D97"/>
+  <dimension ref="A1:D69"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -460,16 +460,16 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>6</v>
+        <v>87</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>art org, projects, arts</t>
+          <t>work, gallery, cultural, arts, young</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Artistic collaboration and open dialogue foster creativity and cultural exchange.</t>
+          <t>No summary available</t>
         </is>
       </c>
     </row>
@@ -478,16 +478,16 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>pierre, mainly, spaces art, steps, italy</t>
+          <t>madrid, amsterdam, territory, experimentation, contemporary art projects</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Artists and cultural workers collaborate to engage communities through creative initiatives.</t>
+          <t>No summary available</t>
         </is>
       </c>
     </row>
@@ -496,16 +496,16 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>century, paintings, museum, concrete, houses</t>
+          <t>houses, city, century, concrete, CITY</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Artist-run spaces foster unique, community-driven contemporary art experiences.</t>
+          <t>No summary available</t>
         </is>
       </c>
     </row>
@@ -514,16 +514,16 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>fashion, press, poetry, took, presented</t>
+          <t>days, existence, subject, CITY, jean</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Artists collaborate to create and promote experimental contemporary art and community engagement.</t>
+          <t>No summary available</t>
         </is>
       </c>
     </row>
@@ -532,16 +532,16 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>popular, going, editions, narrative, submissions</t>
+          <t>stands, turned, project space, wanted, related</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Collaboration and shared creativity thrive in budget-free, non-commercial artistic environments</t>
+          <t>No summary available</t>
         </is>
       </c>
     </row>
@@ -554,12 +554,12 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>club, brussels, stone, wood, group</t>
+          <t>self, collection, joint, ateliers, different</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Art evolves through community engagement and diverse, adaptive platforms.</t>
+          <t>No summary available</t>
         </is>
       </c>
     </row>
@@ -572,12 +572,12 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>artists space, critical, york, discourse, territory</t>
+          <t>generator, square, north, designs, apartment</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Artistic communities and institutions foster creativity and cultural growth.</t>
+          <t>No summary available</t>
         </is>
       </c>
     </row>
@@ -586,16 +586,16 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>filliou, fluxus, shop, adrian, surface</t>
+          <t>diversity, crisis, artistes, press, water</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Art defied oppressive cultural policies through underground networks and documentation.</t>
+          <t>No summary available</t>
         </is>
       </c>
     </row>
@@ -604,16 +604,16 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>music, hall, areas, important, private</t>
+          <t>house, natural, image, step, denis</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Art fosters community engagement and social change through accessible, experimental expression.</t>
+          <t>No summary available</t>
         </is>
       </c>
     </row>
@@ -622,16 +622,16 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>france, laurence, commission, fiction, beautiful</t>
+          <t>poetry, milan, going, tool, art spaces</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Artists from diverse backgrounds collaborate to create and exchange interdisciplinary, transcultural works</t>
+          <t>No summary available</t>
         </is>
       </c>
     </row>
@@ -644,12 +644,12 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>kunstverein, son, editors, non profit organization, city</t>
+          <t>atelier, print, artist centre, techniques, technologies</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>The project emphasizes community-driven information sharing and cultural preservation for collective growth.</t>
+          <t>No summary available</t>
         </is>
       </c>
     </row>
@@ -658,16 +658,16 @@
         <v>11</v>
       </c>
       <c r="B13" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>atelier, exhibition organized, exhibitions artists, michel, damien</t>
+          <t>day day, children, day, pauline, designs</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Artistic communities foster growth, collaboration, and public engagement throughout creative careers.</t>
+          <t>No summary available</t>
         </is>
       </c>
     </row>
@@ -676,16 +676,16 @@
         <v>12</v>
       </c>
       <c r="B14" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>free, athens, enterprise, artistic creation, creations</t>
+          <t>red, art studio, contemporary artists, artist centre, things</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Artistic spaces foster community and discourse by blending personal, public, and institutional</t>
+          <t>No summary available</t>
         </is>
       </c>
     </row>
@@ -694,16 +694,16 @@
         <v>13</v>
       </c>
       <c r="B15" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>commissions, brussels, critics, opening, gallery</t>
+          <t>fellowship, infrastructure, quebec, contexts, organization</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Art and culture can transform and connect communities through collaborative, long-term initiatives.</t>
+          <t>No summary available</t>
         </is>
       </c>
     </row>
@@ -712,16 +712,16 @@
         <v>14</v>
       </c>
       <c r="B16" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>poetry, milan, sale, del, visual</t>
+          <t>marc, factory, lee, weeks, aimed</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Art and creativity thrive in shared, accessible, and affordable community spaces.</t>
+          <t>No summary available</t>
         </is>
       </c>
     </row>
@@ -730,16 +730,16 @@
         <v>15</v>
       </c>
       <c r="B17" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>fine arts, underground, academy, gallery, intermedia</t>
+          <t>works art, archive, academy, summer, fields</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Artistic collectives transform spaces into dynamic cultural hubs.</t>
+          <t>No summary available</t>
         </is>
       </c>
     </row>
@@ -748,16 +748,16 @@
         <v>16</v>
       </c>
       <c r="B18" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>madrid, amsterdam, independent space, artistic research, articles</t>
+          <t>public space, night, alternative, streets, window</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Artists use radio to foster dialogue, share experiences, and explore contemporary creative</t>
+          <t>No summary available</t>
         </is>
       </c>
     </row>
@@ -766,16 +766,16 @@
         <v>17</v>
       </c>
       <c r="B19" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>fellowship, infrastructure, art city, contexts, organization</t>
+          <t>practice, project space, master, tim, design</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Art bridges social divides through community-engaged creative endeavors.</t>
+          <t>No summary available</t>
         </is>
       </c>
     </row>
@@ -784,16 +784,16 @@
         <v>18</v>
       </c>
       <c r="B20" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>lyon, moved, street, studio, supporting</t>
+          <t>short, everyday, hundreds artists, rented, conventional</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Artists find collective purpose through shared space and collaborative exhibitions.</t>
+          <t>No summary available</t>
         </is>
       </c>
     </row>
@@ -802,16 +802,16 @@
         <v>19</v>
       </c>
       <c r="B21" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>media, archive, society, online, hub</t>
+          <t>artists art, months, production, collaboration, school environment</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Contemporary art fosters global exchange and community engagement through diverse exhibitions and publications</t>
+          <t>No summary available</t>
         </is>
       </c>
     </row>
@@ -820,16 +820,16 @@
         <v>20</v>
       </c>
       <c r="B22" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>recent years, turned, regularly, academy, constantly</t>
+          <t>residencies, programme, organisations, based artists, london</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Community spaces foster artistic and technological innovation over time.</t>
+          <t>No summary available</t>
         </is>
       </c>
     </row>
@@ -842,12 +842,12 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>film, known, buy, materials, resident</t>
+          <t>creativity, science, foundation, premises, research</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Artistic expression thrives in small, adaptable spaces through varied media.</t>
+          <t>No summary available</t>
         </is>
       </c>
     </row>
@@ -860,12 +860,12 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>created, curatorial, seven, europe, brussels</t>
+          <t>press, took, presented, archives, series</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Art supports and connects artists, fostering their growth and societal impact.</t>
+          <t>No summary available</t>
         </is>
       </c>
     </row>
@@ -878,12 +878,12 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>vienna, creates, community, art org, environment</t>
+          <t>laboratory, articles, like, street, spaces</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Artistic spaces foster creativity, community, and diverse contemporary art experiences.</t>
+          <t>No summary available</t>
         </is>
       </c>
     </row>
@@ -896,12 +896,12 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>visual artists, wine, practice, international, remarkable</t>
+          <t>organization, laboratory, video, stations, supported</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Contemporary art fosters community engagement and cultural exchange.</t>
+          <t>No summary available</t>
         </is>
       </c>
     </row>
@@ -914,12 +914,12 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>contemporary creation, plastic, today, follows, micro</t>
+          <t>appreciation, contemporary visual, lived, response, generation</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>The text explores the intersection of visual arts and literature through collaborative spaces and interdisciplinary</t>
+          <t>No summary available</t>
         </is>
       </c>
     </row>
@@ -928,16 +928,16 @@
         <v>26</v>
       </c>
       <c r="B28" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>michele, diversity, charlie, crisis, contemporary artists</t>
+          <t>location, meanings, experimental projects, stages, disciplines arts</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Art can transform and revitalize neglected urban spaces through community engagement and free access</t>
+          <t>No summary available</t>
         </is>
       </c>
     </row>
@@ -946,16 +946,16 @@
         <v>27</v>
       </c>
       <c r="B29" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>organization, video, stations, supported, worldwide</t>
+          <t>australia, expanded, exhibiting, england, studio</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>Contemporary art challenges traditional roles and formats to foster dialogue and experimentation.</t>
+          <t>No summary available</t>
         </is>
       </c>
     </row>
@@ -964,16 +964,16 @@
         <v>28</v>
       </c>
       <c r="B30" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>project space, meters, big, different artistic, building</t>
+          <t>fashion, germany, south, exhibited, downtown</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>Artists drive cultural innovation through collaborative, multi-disciplinary projects.</t>
+          <t>No summary available</t>
         </is>
       </c>
     </row>
@@ -982,16 +982,16 @@
         <v>29</v>
       </c>
       <c r="B31" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>arts education, communication, want, developing, offer</t>
+          <t>tools, limoges, recent years, academy, recent</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>Art spaces can drive cultural evolution through adaptability and inclusive dialogue.</t>
+          <t>No summary available</t>
         </is>
       </c>
     </row>
@@ -1000,16 +1000,16 @@
         <v>30</v>
       </c>
       <c r="B32" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>romania, artspace, cluj, hungary, countries</t>
+          <t>installed, district, caroline, artists installed, union</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>Artistic collaboration fosters innovative, socially engaged public art projects.</t>
+          <t>No summary available</t>
         </is>
       </c>
     </row>
@@ -1018,16 +1018,16 @@
         <v>31</v>
       </c>
       <c r="B33" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>intervention, intention, contributing, interventions, george</t>
+          <t>vienna, participated, gallery, limited, dedicated</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>Artistic spaces foster creative exploration, collaboration, and community engagement.</t>
+          <t>No summary available</t>
         </is>
       </c>
     </row>
@@ -1036,16 +1036,16 @@
         <v>32</v>
       </c>
       <c r="B34" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>children, dijon, workshop, seven, evolved</t>
+          <t>commission, production structure, shares, interdisciplinary art, union</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>Art fosters community engagement and personal expression through accessible creative spaces.</t>
+          <t>No summary available</t>
         </is>
       </c>
     </row>
@@ -1054,16 +1054,16 @@
         <v>33</v>
       </c>
       <c r="B35" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>production, artists commissioners, rock, companies, student</t>
+          <t>committee, transmission, glasgow, michael, standard</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>Art spaces foster creativity, collaboration, and dialogue among artists.</t>
+          <t>No summary available</t>
         </is>
       </c>
     </row>
@@ -1072,16 +1072,16 @@
         <v>34</v>
       </c>
       <c r="B36" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>current art, public space, purpose, jean, experiment</t>
+          <t>discover, service, multidisciplinary, sound, monthly</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>Art supports innovation and challenges societal norms when given freedom and resources.</t>
+          <t>No summary available</t>
         </is>
       </c>
     </row>
@@ -1090,16 +1090,16 @@
         <v>35</v>
       </c>
       <c r="B37" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>laboratory, like, spaces, rhythm, moment</t>
+          <t>opening, thirty, association aims, artists invited, recording</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>Art fosters global dialogue and supports local artists amidst changing cultural landscapes.</t>
+          <t>No summary available</t>
         </is>
       </c>
     </row>
@@ -1108,16 +1108,16 @@
         <v>36</v>
       </c>
       <c r="B38" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>western, interdisciplinary, media, experimental art, practices</t>
+          <t>editors, non profit organization, profit organization, history, northern</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>Art fosters collaboration and direct engagement between creators and audiences.</t>
+          <t>No summary available</t>
         </is>
       </c>
     </row>
@@ -1126,16 +1126,16 @@
         <v>37</v>
       </c>
       <c r="B39" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>natural, step, river, steps, encourages</t>
+          <t>family, born, annual exhibitions, exhibitions conferences, body</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>Contemporary arts foster societal awareness and dialogue through diverse, experimental, and accessible</t>
+          <t>No summary available</t>
         </is>
       </c>
     </row>
@@ -1144,16 +1144,16 @@
         <v>38</v>
       </c>
       <c r="B40" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>pauline, designs, production, self, divided</t>
+          <t>systems, amsterdam, residential, relationships, organizing</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>Art challenges traditional museum formats to embrace diverse, interactive experiences.</t>
+          <t>No summary available</t>
         </is>
       </c>
     </row>
@@ -1162,16 +1162,16 @@
         <v>39</v>
       </c>
       <c r="B41" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>artist art, currently, associative, independent exhibition, painting video</t>
+          <t>exhibition organized, exhibitions artists, damien, james, format</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>Artists collaborate to create shared spaces for experimentation and collective creation.</t>
+          <t>No summary available</t>
         </is>
       </c>
     </row>
@@ -1180,16 +1180,16 @@
         <v>40</v>
       </c>
       <c r="B42" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>tools, limoges, association, promotes, stay</t>
+          <t>extended, pauline, houses, gallery, opening</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>Artists collectively challenged traditional boundaries through interdisciplinary experimentation.</t>
+          <t>No summary available</t>
         </is>
       </c>
     </row>
@@ -1198,16 +1198,16 @@
         <v>41</v>
       </c>
       <c r="B43" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>station, nice, service, drawings, build</t>
+          <t>wishes, residency, studio, weeks, artist residency</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>Emerging artists, especially women, are championed and given platforms to showcase</t>
+          <t>No summary available</t>
         </is>
       </c>
     </row>
@@ -1216,16 +1216,16 @@
         <v>42</v>
       </c>
       <c r="B44" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>factory, lee, exhibition area, art org, young artists</t>
+          <t>laurence, france, fiction, beautiful, marc</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>A collaborative, interdisciplinary space fosters artistic creation and community engagement.</t>
+          <t>No summary available</t>
         </is>
       </c>
     </row>
@@ -1234,16 +1234,16 @@
         <v>43</v>
       </c>
       <c r="B45" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>rooms, project space, reception, limoges, visiting</t>
+          <t>ground, architecture, artist space, art area, diffusion contemporary</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>Art fosters community and innovation through shared, inclusive, and experimental spaces.</t>
+          <t>No summary available</t>
         </is>
       </c>
     </row>
@@ -1252,16 +1252,16 @@
         <v>44</v>
       </c>
       <c r="B46" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>public space, rented, conventional, alternative, interior</t>
+          <t>encounters, stop, biennial, wish, dan</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>Art and absurdity intersect to explore everyday life and marginal history.</t>
+          <t>No summary available</t>
         </is>
       </c>
     </row>
@@ -1270,16 +1270,16 @@
         <v>45</v>
       </c>
       <c r="B47" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>house, denis, gives, researchers, housing</t>
+          <t>works art, photography, outside, planned, art media</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>The text describes organizations fostering artistic creation, education, and cultural exchange through</t>
+          <t>No summary available</t>
         </is>
       </c>
     </row>
@@ -1288,16 +1288,16 @@
         <v>46</v>
       </c>
       <c r="B48" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>self, collection, ateliers, managed, physical</t>
+          <t>surface, adrian, damien, created artists, artists based</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>Art galleries can transform public spaces and foster emerging artists' growth.</t>
+          <t>No summary available</t>
         </is>
       </c>
     </row>
@@ -1306,16 +1306,16 @@
         <v>47</v>
       </c>
       <c r="B49" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>ground, artist space, like minded, encourage dialogue, easily</t>
+          <t>lab, thing, sharing, created, need</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>Art fosters community growth and professional development through diverse, experimental programs.</t>
+          <t>No summary available</t>
         </is>
       </c>
     </row>
@@ -1328,12 +1328,12 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>work work, employment, day day, france, laurent</t>
+          <t>steps, situated, mainly, space intended, limits</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>Collaboration and adaptability drive innovative artistic expression and growth.</t>
+          <t>No summary available</t>
         </is>
       </c>
     </row>
@@ -1346,12 +1346,12 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>situ, tim, objects, october, growing</t>
+          <t>graphic, graphic design, brussels, french, university</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>Contemporary art thrives through diverse media and independent artist-driven spaces.</t>
+          <t>No summary available</t>
         </is>
       </c>
     </row>
@@ -1364,12 +1364,12 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>projets, avant, garde, doors, space non</t>
+          <t>italy, artist space, space composed, athens, happenings</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>Artists collaborate to challenge conventions and foster dialogue through collective efforts.</t>
+          <t>No summary available</t>
         </is>
       </c>
     </row>
@@ -1382,12 +1382,12 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>contemporary artists, exhibition hall, canada, artist centre, documentation</t>
+          <t>opening, artists present work, dedicated contemporary creation, dedicated exhibition, exchange</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>Artistic collaboration and community engagement foster creative growth.</t>
+          <t>No summary available</t>
         </is>
       </c>
     </row>
@@ -1400,12 +1400,12 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>profit artist centre, canadian, gallery space, festival, director</t>
+          <t>dijon, workshop, seven, school, area</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>Artists collaborate and create in shared, independent studio spaces dedicated to both work</t>
+          <t>No summary available</t>
         </is>
       </c>
     </row>
@@ -1418,12 +1418,12 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>residencies, australia, programme, international, organisations</t>
+          <t>documents, contributions, museum, video, wide range</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>The text emphasizes fostering contemporary art through experimental spaces and supportive programs.</t>
+          <t>No summary available</t>
         </is>
       </c>
     </row>
@@ -1436,12 +1436,12 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>generator, way, life, remains, existence</t>
+          <t>solo, lieu, common, levels, club</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>Art champions experimental creativity and accessibility for all artists.</t>
+          <t>No summary available</t>
         </is>
       </c>
     </row>
@@ -1454,12 +1454,12 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>current art, city city, centre, designs, quebec</t>
+          <t>narrative, question, object, opens, volume</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>Emerging artists and innovative art forms are fostered through collaborative, non-h</t>
+          <t>No summary available</t>
         </is>
       </c>
     </row>
@@ -1472,12 +1472,12 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>residences, individual, england, responsible, collective exhibitions</t>
+          <t>audio, legendary, york, matta, gordon matta clark</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>Artists collaborate and exhibit in shared, accessible spaces to foster creativity and community</t>
+          <t>No summary available</t>
         </is>
       </c>
     </row>
@@ -1490,12 +1490,12 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>association, promotion, communication, meetings discussions, artists institutions</t>
+          <t>submissions, art city, canada, accessible, programming</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>Artists transform personal spaces into intimate, unconventional exhibition environments.</t>
+          <t>No summary available</t>
         </is>
       </c>
     </row>
@@ -1508,12 +1508,12 @@
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>artspace, communities, street, centres, current</t>
+          <t>work work, current art, work, france, centre</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>Community-driven art fosters local engagement and multidisciplinary creativity.</t>
+          <t>No summary available</t>
         </is>
       </c>
     </row>
@@ -1526,12 +1526,12 @@
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>laurence, king, beaux arts, school, artist work</t>
+          <t>wood, stone, thomas, decided, atelier</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>Collectives maximize their skills and resources for collaborative artistic and cultural projects.</t>
+          <t>No summary available</t>
         </is>
       </c>
     </row>
@@ -1544,12 +1544,12 @@
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>committed, performance space, thinkers, artists contemporary, brazilian</t>
+          <t>film screenings, activities, film, curating, document</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>Artistic experimentation and community engagement through adaptable exhibition spaces.</t>
+          <t>No summary available</t>
         </is>
       </c>
     </row>
@@ -1562,12 +1562,12 @@
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>square, north, district, factory, art architecture</t>
+          <t>artist project, discursive, cultivate, photo, chicago</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>Artistic spaces foster creativity through temporary, interconnected, and precarious networks.</t>
+          <t>No summary available</t>
         </is>
       </c>
     </row>
@@ -1580,12 +1580,12 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>gallery, south, steel, artiste, berlinian</t>
+          <t>western, program, melbourne, interdisciplinary, experimental art</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>Experimental art fosters interdisciplinary creativity and innovation.</t>
+          <t>No summary available</t>
         </is>
       </c>
     </row>
@@ -1598,12 +1598,12 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>experimentation, celebrated, universe, combines, innovation</t>
+          <t>young emerging, melbourne, broader, gallery, young emerging artists</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>Art fosters interdisciplinary exploration and continuous evolution.</t>
+          <t>No summary available</t>
         </is>
       </c>
     </row>
@@ -1616,12 +1616,12 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>installed, district, caroline, union, artists production</t>
+          <t>pierre, hong, central, art institutions, spaces art</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>Printed art is promoted as an accessible, interactive, and evolving medium.</t>
+          <t>No summary available</t>
         </is>
       </c>
     </row>
@@ -1634,12 +1634,12 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>stands, wanted, helps, continuously, exists</t>
+          <t>hall, purposes, purpose, allows, passed</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>Artists collaboratively transform and utilize shared spaces for creative expression and learning.</t>
+          <t>No summary available</t>
         </is>
       </c>
     </row>
@@ -1652,12 +1652,12 @@
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>past, temporal, spatial, double, art space</t>
+          <t>ateliers, association, period, residence, artists particular</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>Artistic collaboration and adaptability foster innovative, site-specific creative dialogues.</t>
+          <t>No summary available</t>
         </is>
       </c>
     </row>
@@ -1670,404 +1670,12 @@
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>art theory, cultivate, stimulating, non, formal</t>
+          <t>music, areas, private, border, important</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>Contemporary art thrives in unconventional, adaptable spaces.</t>
-        </is>
-      </c>
-    </row>
-    <row r="70">
-      <c r="A70" t="n">
-        <v>68</v>
-      </c>
-      <c r="B70" t="n">
-        <v>2</v>
-      </c>
-      <c r="C70" t="inlineStr"/>
-      <c r="D70" t="inlineStr">
-        <is>
-          <t>No summary available.</t>
-        </is>
-      </c>
-    </row>
-    <row r="71">
-      <c r="A71" t="n">
-        <v>69</v>
-      </c>
-      <c r="B71" t="n">
-        <v>2</v>
-      </c>
-      <c r="C71" t="inlineStr"/>
-      <c r="D71" t="inlineStr">
-        <is>
-          <t>No summary available.</t>
-        </is>
-      </c>
-    </row>
-    <row r="72">
-      <c r="A72" t="n">
-        <v>70</v>
-      </c>
-      <c r="B72" t="n">
-        <v>2</v>
-      </c>
-      <c r="C72" t="inlineStr"/>
-      <c r="D72" t="inlineStr">
-        <is>
-          <t>No summary available.</t>
-        </is>
-      </c>
-    </row>
-    <row r="73">
-      <c r="A73" t="n">
-        <v>71</v>
-      </c>
-      <c r="B73" t="n">
-        <v>2</v>
-      </c>
-      <c r="C73" t="inlineStr"/>
-      <c r="D73" t="inlineStr">
-        <is>
-          <t>No summary available.</t>
-        </is>
-      </c>
-    </row>
-    <row r="74">
-      <c r="A74" t="n">
-        <v>72</v>
-      </c>
-      <c r="B74" t="n">
-        <v>2</v>
-      </c>
-      <c r="C74" t="inlineStr"/>
-      <c r="D74" t="inlineStr">
-        <is>
-          <t>No summary available.</t>
-        </is>
-      </c>
-    </row>
-    <row r="75">
-      <c r="A75" t="n">
-        <v>73</v>
-      </c>
-      <c r="B75" t="n">
-        <v>2</v>
-      </c>
-      <c r="C75" t="inlineStr"/>
-      <c r="D75" t="inlineStr">
-        <is>
-          <t>No summary available.</t>
-        </is>
-      </c>
-    </row>
-    <row r="76">
-      <c r="A76" t="n">
-        <v>74</v>
-      </c>
-      <c r="B76" t="n">
-        <v>2</v>
-      </c>
-      <c r="C76" t="inlineStr"/>
-      <c r="D76" t="inlineStr">
-        <is>
-          <t>No summary available.</t>
-        </is>
-      </c>
-    </row>
-    <row r="77">
-      <c r="A77" t="n">
-        <v>75</v>
-      </c>
-      <c r="B77" t="n">
-        <v>2</v>
-      </c>
-      <c r="C77" t="inlineStr"/>
-      <c r="D77" t="inlineStr">
-        <is>
-          <t>No summary available.</t>
-        </is>
-      </c>
-    </row>
-    <row r="78">
-      <c r="A78" t="n">
-        <v>76</v>
-      </c>
-      <c r="B78" t="n">
-        <v>2</v>
-      </c>
-      <c r="C78" t="inlineStr"/>
-      <c r="D78" t="inlineStr">
-        <is>
-          <t>No summary available.</t>
-        </is>
-      </c>
-    </row>
-    <row r="79">
-      <c r="A79" t="n">
-        <v>77</v>
-      </c>
-      <c r="B79" t="n">
-        <v>2</v>
-      </c>
-      <c r="C79" t="inlineStr"/>
-      <c r="D79" t="inlineStr">
-        <is>
-          <t>No summary available.</t>
-        </is>
-      </c>
-    </row>
-    <row r="80">
-      <c r="A80" t="n">
-        <v>78</v>
-      </c>
-      <c r="B80" t="n">
-        <v>2</v>
-      </c>
-      <c r="C80" t="inlineStr"/>
-      <c r="D80" t="inlineStr">
-        <is>
-          <t>No summary available.</t>
-        </is>
-      </c>
-    </row>
-    <row r="81">
-      <c r="A81" t="n">
-        <v>79</v>
-      </c>
-      <c r="B81" t="n">
-        <v>2</v>
-      </c>
-      <c r="C81" t="inlineStr"/>
-      <c r="D81" t="inlineStr">
-        <is>
-          <t>No summary available.</t>
-        </is>
-      </c>
-    </row>
-    <row r="82">
-      <c r="A82" t="n">
-        <v>80</v>
-      </c>
-      <c r="B82" t="n">
-        <v>2</v>
-      </c>
-      <c r="C82" t="inlineStr"/>
-      <c r="D82" t="inlineStr">
-        <is>
-          <t>No summary available.</t>
-        </is>
-      </c>
-    </row>
-    <row r="83">
-      <c r="A83" t="n">
-        <v>81</v>
-      </c>
-      <c r="B83" t="n">
-        <v>2</v>
-      </c>
-      <c r="C83" t="inlineStr"/>
-      <c r="D83" t="inlineStr">
-        <is>
-          <t>No summary available.</t>
-        </is>
-      </c>
-    </row>
-    <row r="84">
-      <c r="A84" t="n">
-        <v>82</v>
-      </c>
-      <c r="B84" t="n">
-        <v>2</v>
-      </c>
-      <c r="C84" t="inlineStr"/>
-      <c r="D84" t="inlineStr">
-        <is>
-          <t>No summary available.</t>
-        </is>
-      </c>
-    </row>
-    <row r="85">
-      <c r="A85" t="n">
-        <v>83</v>
-      </c>
-      <c r="B85" t="n">
-        <v>2</v>
-      </c>
-      <c r="C85" t="inlineStr"/>
-      <c r="D85" t="inlineStr">
-        <is>
-          <t>No summary available.</t>
-        </is>
-      </c>
-    </row>
-    <row r="86">
-      <c r="A86" t="n">
-        <v>84</v>
-      </c>
-      <c r="B86" t="n">
-        <v>2</v>
-      </c>
-      <c r="C86" t="inlineStr"/>
-      <c r="D86" t="inlineStr">
-        <is>
-          <t>No summary available.</t>
-        </is>
-      </c>
-    </row>
-    <row r="87">
-      <c r="A87" t="n">
-        <v>85</v>
-      </c>
-      <c r="B87" t="n">
-        <v>2</v>
-      </c>
-      <c r="C87" t="inlineStr"/>
-      <c r="D87" t="inlineStr">
-        <is>
-          <t>No summary available.</t>
-        </is>
-      </c>
-    </row>
-    <row r="88">
-      <c r="A88" t="n">
-        <v>86</v>
-      </c>
-      <c r="B88" t="n">
-        <v>2</v>
-      </c>
-      <c r="C88" t="inlineStr"/>
-      <c r="D88" t="inlineStr">
-        <is>
-          <t>No summary available.</t>
-        </is>
-      </c>
-    </row>
-    <row r="89">
-      <c r="A89" t="n">
-        <v>87</v>
-      </c>
-      <c r="B89" t="n">
-        <v>2</v>
-      </c>
-      <c r="C89" t="inlineStr"/>
-      <c r="D89" t="inlineStr">
-        <is>
-          <t>No summary available.</t>
-        </is>
-      </c>
-    </row>
-    <row r="90">
-      <c r="A90" t="n">
-        <v>88</v>
-      </c>
-      <c r="B90" t="n">
-        <v>2</v>
-      </c>
-      <c r="C90" t="inlineStr"/>
-      <c r="D90" t="inlineStr">
-        <is>
-          <t>No summary available.</t>
-        </is>
-      </c>
-    </row>
-    <row r="91">
-      <c r="A91" t="n">
-        <v>89</v>
-      </c>
-      <c r="B91" t="n">
-        <v>2</v>
-      </c>
-      <c r="C91" t="inlineStr"/>
-      <c r="D91" t="inlineStr">
-        <is>
-          <t>No summary available.</t>
-        </is>
-      </c>
-    </row>
-    <row r="92">
-      <c r="A92" t="n">
-        <v>90</v>
-      </c>
-      <c r="B92" t="n">
-        <v>2</v>
-      </c>
-      <c r="C92" t="inlineStr"/>
-      <c r="D92" t="inlineStr">
-        <is>
-          <t>No summary available.</t>
-        </is>
-      </c>
-    </row>
-    <row r="93">
-      <c r="A93" t="n">
-        <v>91</v>
-      </c>
-      <c r="B93" t="n">
-        <v>2</v>
-      </c>
-      <c r="C93" t="inlineStr"/>
-      <c r="D93" t="inlineStr">
-        <is>
-          <t>No summary available.</t>
-        </is>
-      </c>
-    </row>
-    <row r="94">
-      <c r="A94" t="n">
-        <v>92</v>
-      </c>
-      <c r="B94" t="n">
-        <v>2</v>
-      </c>
-      <c r="C94" t="inlineStr"/>
-      <c r="D94" t="inlineStr">
-        <is>
-          <t>No summary available.</t>
-        </is>
-      </c>
-    </row>
-    <row r="95">
-      <c r="A95" t="n">
-        <v>93</v>
-      </c>
-      <c r="B95" t="n">
-        <v>2</v>
-      </c>
-      <c r="C95" t="inlineStr"/>
-      <c r="D95" t="inlineStr">
-        <is>
-          <t>No summary available.</t>
-        </is>
-      </c>
-    </row>
-    <row r="96">
-      <c r="A96" t="n">
-        <v>94</v>
-      </c>
-      <c r="B96" t="n">
-        <v>2</v>
-      </c>
-      <c r="C96" t="inlineStr"/>
-      <c r="D96" t="inlineStr">
-        <is>
-          <t>No summary available.</t>
-        </is>
-      </c>
-    </row>
-    <row r="97">
-      <c r="A97" t="n">
-        <v>95</v>
-      </c>
-      <c r="B97" t="n">
-        <v>2</v>
-      </c>
-      <c r="C97" t="inlineStr"/>
-      <c r="D97" t="inlineStr">
-        <is>
-          <t>No summary available.</t>
+          <t>No summary available</t>
         </is>
       </c>
     </row>

</xml_diff>